<commit_message>
update the excel spreadsheet
</commit_message>
<xml_diff>
--- a/segmentConstraints.xlsx
+++ b/segmentConstraints.xlsx
@@ -11,9 +11,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
-  <si>
-    <t>Table 1</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="32">
+  <si>
+    <t>Parameter</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Column2</t>
+  </si>
+  <si>
+    <t>Column3</t>
+  </si>
+  <si>
+    <t>Column4</t>
+  </si>
+  <si>
+    <t>Column5</t>
+  </si>
+  <si>
+    <t>Column6</t>
+  </si>
+  <si>
+    <t>Column7</t>
+  </si>
+  <si>
+    <t>Column8</t>
+  </si>
+  <si>
+    <t>Column9</t>
+  </si>
+  <si>
+    <t>Column10</t>
+  </si>
+  <si>
+    <t>Column11</t>
   </si>
   <si>
     <t>stroke</t>
@@ -80,7 +116,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -92,13 +128,18 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
+      <sz val="15"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <b val="1"/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -114,6 +155,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="11"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="12"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -147,21 +194,21 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
@@ -172,16 +219,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -204,6 +248,7 @@
       <rgbColor rgb="ffd5d5d5"/>
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff5e5e5e"/>
+      <rgbColor rgb="ffffffff"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -220,10 +265,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="5E5E5E"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="D5D5D5"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="00A2FF"/>
@@ -400,11 +445,14 @@
     <a:spDef>
       <a:spPr>
         <a:solidFill>
-          <a:srgbClr val="000000"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -413,33 +461,33 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="584200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="Helvetica Neue Medium"/>
-            <a:ea typeface="Helvetica Neue Medium"/>
-            <a:cs typeface="Helvetica Neue Medium"/>
-            <a:sym typeface="Helvetica Neue Medium"/>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -678,12 +726,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -964,7 +1012,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1232,647 +1280,666 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:M16"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="10.0781" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.0781" style="1" customWidth="1"/>
-    <col min="3" max="10" width="16.9609" style="1" customWidth="1"/>
-    <col min="11" max="13" width="16.1641" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1719" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.1719" style="1" customWidth="1"/>
+    <col min="3" max="10" width="17" style="1" customWidth="1"/>
+    <col min="11" max="13" width="16.1719" style="1" customWidth="1"/>
     <col min="14" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27.65" customHeight="1">
+    <row r="1" ht="20.05" customHeight="1">
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
+      <c r="B1" t="s" s="2">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s" s="3">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s" s="3">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s" s="3">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s" s="3">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s" s="3">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s" s="3">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s" s="3">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s" s="3">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s" s="3">
+        <v>12</v>
+      </c>
     </row>
     <row r="2" ht="20.05" customHeight="1">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" t="s" s="4">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s" s="4">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s" s="4">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s" s="4">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s" s="4">
-        <v>1</v>
-      </c>
-      <c r="H2" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="I2" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="J2" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="K2" t="s" s="4">
-        <v>3</v>
-      </c>
-      <c r="L2" t="s" s="4">
-        <v>4</v>
-      </c>
-      <c r="M2" t="s" s="4">
-        <v>5</v>
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" t="s" s="3">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s" s="3">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s" s="3">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s" s="3">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s" s="3">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s" s="3">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s" s="3">
+        <v>14</v>
+      </c>
+      <c r="J2" t="s" s="3">
+        <v>14</v>
+      </c>
+      <c r="K2" t="s" s="3">
+        <v>15</v>
+      </c>
+      <c r="L2" t="s" s="3">
+        <v>16</v>
+      </c>
+      <c r="M2" t="s" s="3">
+        <v>17</v>
       </c>
     </row>
     <row r="3" ht="20.05" customHeight="1">
-      <c r="A3" s="3"/>
+      <c r="A3" s="4"/>
       <c r="B3" s="5"/>
       <c r="C3" t="s" s="6">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s" s="6">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="E3" t="s" s="6">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="F3" t="s" s="6">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="G3" t="s" s="6">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="H3" t="s" s="6">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="I3" t="s" s="6">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="J3" t="s" s="6">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="K3" t="s" s="6">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="L3" t="s" s="6">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="M3" s="7"/>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" t="s" s="8">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s" s="10">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s" s="10">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s" s="10">
-        <v>15</v>
-      </c>
-      <c r="F4" t="s" s="10">
-        <v>15</v>
-      </c>
-      <c r="G4" t="s" s="10">
-        <v>15</v>
-      </c>
-      <c r="H4" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="I4" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="J4" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="K4" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="L4" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="M4" t="s" s="11">
-        <v>17</v>
+      <c r="A4" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s" s="8">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s" s="9">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s" s="9">
+        <v>27</v>
+      </c>
+      <c r="E4" t="s" s="9">
+        <v>27</v>
+      </c>
+      <c r="F4" t="s" s="9">
+        <v>27</v>
+      </c>
+      <c r="G4" t="s" s="9">
+        <v>27</v>
+      </c>
+      <c r="H4" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="I4" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="J4" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="K4" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="L4" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="M4" t="s" s="10">
+        <v>29</v>
       </c>
     </row>
     <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" t="s" s="8">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s" s="9">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s" s="10">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s" s="10">
-        <v>15</v>
-      </c>
-      <c r="E5" t="s" s="10">
-        <v>15</v>
-      </c>
-      <c r="F5" t="s" s="10">
-        <v>15</v>
-      </c>
-      <c r="G5" t="s" s="10">
-        <v>15</v>
-      </c>
-      <c r="H5" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="I5" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="J5" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="K5" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="L5" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="M5" t="s" s="11">
-        <v>17</v>
+      <c r="A5" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s" s="8">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s" s="9">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s" s="9">
+        <v>27</v>
+      </c>
+      <c r="E5" t="s" s="9">
+        <v>27</v>
+      </c>
+      <c r="F5" t="s" s="9">
+        <v>27</v>
+      </c>
+      <c r="G5" t="s" s="9">
+        <v>27</v>
+      </c>
+      <c r="H5" t="s" s="10">
+        <v>29</v>
+      </c>
+      <c r="I5" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="J5" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="K5" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="L5" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="M5" t="s" s="10">
+        <v>29</v>
       </c>
     </row>
     <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" t="s" s="8">
-        <v>1</v>
-      </c>
-      <c r="B6" t="s" s="9">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s" s="10">
-        <v>15</v>
-      </c>
-      <c r="D6" t="s" s="10">
-        <v>15</v>
-      </c>
-      <c r="E6" t="s" s="10">
-        <v>15</v>
-      </c>
-      <c r="F6" t="s" s="10">
-        <v>15</v>
-      </c>
-      <c r="G6" t="s" s="10">
-        <v>15</v>
-      </c>
-      <c r="H6" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="I6" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="J6" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="K6" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="L6" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="M6" t="s" s="11">
-        <v>17</v>
+      <c r="A6" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s" s="8">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s" s="9">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s" s="9">
+        <v>27</v>
+      </c>
+      <c r="E6" t="s" s="9">
+        <v>27</v>
+      </c>
+      <c r="F6" t="s" s="9">
+        <v>27</v>
+      </c>
+      <c r="G6" t="s" s="9">
+        <v>27</v>
+      </c>
+      <c r="H6" t="s" s="10">
+        <v>29</v>
+      </c>
+      <c r="I6" t="s" s="10">
+        <v>29</v>
+      </c>
+      <c r="J6" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="K6" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="L6" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="M6" t="s" s="10">
+        <v>29</v>
       </c>
     </row>
     <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" t="s" s="8">
-        <v>1</v>
-      </c>
-      <c r="B7" t="s" s="9">
-        <v>9</v>
-      </c>
-      <c r="C7" t="s" s="10">
-        <v>15</v>
-      </c>
-      <c r="D7" t="s" s="10">
-        <v>15</v>
-      </c>
-      <c r="E7" t="s" s="10">
-        <v>15</v>
-      </c>
-      <c r="F7" t="s" s="10">
-        <v>15</v>
-      </c>
-      <c r="G7" t="s" s="10">
-        <v>15</v>
-      </c>
-      <c r="H7" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="I7" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="J7" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="K7" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="L7" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="M7" t="s" s="11">
-        <v>17</v>
+      <c r="A7" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s" s="8">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s" s="9">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s" s="9">
+        <v>27</v>
+      </c>
+      <c r="E7" t="s" s="9">
+        <v>27</v>
+      </c>
+      <c r="F7" t="s" s="9">
+        <v>27</v>
+      </c>
+      <c r="G7" t="s" s="9">
+        <v>27</v>
+      </c>
+      <c r="H7" t="s" s="10">
+        <v>29</v>
+      </c>
+      <c r="I7" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="J7" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="K7" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="L7" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="M7" t="s" s="10">
+        <v>29</v>
       </c>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" t="s" s="8">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s" s="9">
-        <v>10</v>
-      </c>
-      <c r="C8" t="s" s="10">
-        <v>15</v>
-      </c>
-      <c r="D8" t="s" s="10">
-        <v>15</v>
-      </c>
-      <c r="E8" t="s" s="10">
-        <v>15</v>
-      </c>
-      <c r="F8" t="s" s="10">
-        <v>15</v>
-      </c>
-      <c r="G8" t="s" s="10">
-        <v>15</v>
-      </c>
-      <c r="H8" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="I8" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="J8" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="K8" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="L8" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="M8" t="s" s="11">
-        <v>17</v>
+      <c r="A8" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s" s="8">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s" s="9">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s" s="9">
+        <v>27</v>
+      </c>
+      <c r="E8" t="s" s="9">
+        <v>27</v>
+      </c>
+      <c r="F8" t="s" s="9">
+        <v>27</v>
+      </c>
+      <c r="G8" t="s" s="9">
+        <v>27</v>
+      </c>
+      <c r="H8" t="s" s="10">
+        <v>29</v>
+      </c>
+      <c r="I8" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="J8" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="K8" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="L8" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="M8" t="s" s="10">
+        <v>29</v>
       </c>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="B9" t="s" s="9">
-        <v>11</v>
-      </c>
-      <c r="C9" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="D9" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="E9" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="F9" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="G9" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="H9" t="s" s="10">
-        <v>15</v>
-      </c>
-      <c r="I9" t="s" s="10">
-        <v>15</v>
-      </c>
-      <c r="J9" t="s" s="10">
-        <v>15</v>
-      </c>
-      <c r="K9" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="L9" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="M9" t="s" s="11">
-        <v>17</v>
+      <c r="A9" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s" s="8">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="D9" t="s" s="10">
+        <v>29</v>
+      </c>
+      <c r="E9" t="s" s="10">
+        <v>29</v>
+      </c>
+      <c r="F9" t="s" s="10">
+        <v>29</v>
+      </c>
+      <c r="G9" t="s" s="10">
+        <v>29</v>
+      </c>
+      <c r="H9" t="s" s="9">
+        <v>27</v>
+      </c>
+      <c r="I9" t="s" s="9">
+        <v>27</v>
+      </c>
+      <c r="J9" t="s" s="9">
+        <v>27</v>
+      </c>
+      <c r="K9" t="s" s="10">
+        <v>29</v>
+      </c>
+      <c r="L9" t="s" s="10">
+        <v>29</v>
+      </c>
+      <c r="M9" t="s" s="10">
+        <v>29</v>
       </c>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="B10" t="s" s="9">
-        <v>12</v>
-      </c>
-      <c r="C10" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="D10" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="E10" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="F10" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="G10" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="H10" t="s" s="10">
-        <v>15</v>
-      </c>
-      <c r="I10" t="s" s="10">
-        <v>15</v>
-      </c>
-      <c r="J10" t="s" s="10">
-        <v>15</v>
-      </c>
-      <c r="K10" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="L10" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="M10" t="s" s="11">
-        <v>17</v>
+      <c r="A10" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s" s="8">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="D10" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="E10" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="F10" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="G10" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="H10" t="s" s="9">
+        <v>27</v>
+      </c>
+      <c r="I10" t="s" s="9">
+        <v>27</v>
+      </c>
+      <c r="J10" t="s" s="9">
+        <v>27</v>
+      </c>
+      <c r="K10" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="L10" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="M10" t="s" s="10">
+        <v>29</v>
       </c>
     </row>
     <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="B11" t="s" s="9">
-        <v>13</v>
-      </c>
-      <c r="C11" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="D11" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="E11" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="F11" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="G11" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="H11" t="s" s="10">
-        <v>15</v>
-      </c>
-      <c r="I11" t="s" s="10">
-        <v>15</v>
-      </c>
-      <c r="J11" t="s" s="10">
-        <v>15</v>
-      </c>
-      <c r="K11" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="L11" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="M11" t="s" s="11">
-        <v>17</v>
+      <c r="A11" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s" s="8">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="D11" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="E11" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="F11" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="G11" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="H11" t="s" s="9">
+        <v>27</v>
+      </c>
+      <c r="I11" t="s" s="9">
+        <v>27</v>
+      </c>
+      <c r="J11" t="s" s="9">
+        <v>27</v>
+      </c>
+      <c r="K11" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="L11" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="M11" t="s" s="10">
+        <v>29</v>
       </c>
     </row>
     <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" t="s" s="8">
-        <v>3</v>
-      </c>
-      <c r="B12" t="s" s="9">
-        <v>14</v>
-      </c>
-      <c r="C12" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="D12" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="E12" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="F12" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="G12" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="H12" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="I12" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="J12" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="K12" t="s" s="10">
+      <c r="A12" t="s" s="2">
         <v>15</v>
       </c>
-      <c r="L12" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="M12" t="s" s="11">
-        <v>17</v>
+      <c r="B12" t="s" s="8">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="D12" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="E12" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="F12" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="G12" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="H12" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="I12" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="J12" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="K12" t="s" s="9">
+        <v>27</v>
+      </c>
+      <c r="L12" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="M12" t="s" s="10">
+        <v>29</v>
       </c>
     </row>
     <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" t="s" s="8">
-        <v>4</v>
-      </c>
-      <c r="B13" t="s" s="9">
-        <v>18</v>
-      </c>
-      <c r="C13" t="s" s="11">
+      <c r="A13" t="s" s="2">
         <v>16</v>
       </c>
-      <c r="D13" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="E13" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="F13" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="G13" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="H13" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="I13" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="J13" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="K13" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="L13" t="s" s="10">
-        <v>15</v>
-      </c>
-      <c r="M13" t="s" s="11">
-        <v>17</v>
+      <c r="B13" t="s" s="8">
+        <v>30</v>
+      </c>
+      <c r="C13" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="D13" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="E13" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="F13" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="G13" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="H13" t="s" s="10">
+        <v>29</v>
+      </c>
+      <c r="I13" t="s" s="10">
+        <v>29</v>
+      </c>
+      <c r="J13" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="K13" t="s" s="10">
+        <v>29</v>
+      </c>
+      <c r="L13" t="s" s="9">
+        <v>27</v>
+      </c>
+      <c r="M13" t="s" s="10">
+        <v>29</v>
       </c>
     </row>
     <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" t="s" s="8">
-        <v>4</v>
-      </c>
-      <c r="B14" t="s" s="9">
-        <v>19</v>
-      </c>
-      <c r="C14" t="s" s="11">
+      <c r="A14" t="s" s="2">
         <v>16</v>
       </c>
-      <c r="D14" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="E14" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="F14" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="G14" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="H14" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="I14" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="J14" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="K14" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="L14" t="s" s="10">
-        <v>15</v>
-      </c>
-      <c r="M14" t="s" s="11">
-        <v>17</v>
+      <c r="B14" t="s" s="8">
+        <v>31</v>
+      </c>
+      <c r="C14" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="D14" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="E14" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="F14" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="G14" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="H14" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="I14" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="J14" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="K14" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="L14" t="s" s="9">
+        <v>27</v>
+      </c>
+      <c r="M14" t="s" s="10">
+        <v>29</v>
       </c>
     </row>
     <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" t="s" s="8">
-        <v>5</v>
-      </c>
-      <c r="B15" t="s" s="9">
-        <v>18</v>
-      </c>
-      <c r="C15" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="D15" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="E15" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="F15" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="G15" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="H15" t="s" s="11">
+      <c r="A15" t="s" s="2">
         <v>17</v>
       </c>
-      <c r="I15" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="J15" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="K15" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="L15" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="M15" t="s" s="10">
-        <v>15</v>
+      <c r="B15" t="s" s="8">
+        <v>30</v>
+      </c>
+      <c r="C15" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="D15" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="E15" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="F15" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="G15" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="H15" t="s" s="10">
+        <v>29</v>
+      </c>
+      <c r="I15" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="J15" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="K15" t="s" s="10">
+        <v>29</v>
+      </c>
+      <c r="L15" t="s" s="10">
+        <v>29</v>
+      </c>
+      <c r="M15" t="s" s="9">
+        <v>27</v>
       </c>
     </row>
     <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" t="s" s="8">
-        <v>5</v>
-      </c>
-      <c r="B16" t="s" s="9">
-        <v>19</v>
-      </c>
-      <c r="C16" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="D16" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="E16" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="F16" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="G16" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="H16" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="I16" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="J16" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="K16" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="L16" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="M16" t="s" s="10">
-        <v>15</v>
+      <c r="A16" t="s" s="2">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s" s="8">
+        <v>31</v>
+      </c>
+      <c r="C16" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="D16" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="E16" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="F16" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="G16" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="H16" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="I16" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="J16" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="K16" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="L16" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="M16" t="s" s="9">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:M1"/>
-  </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>

</xml_diff>

<commit_message>
chaging values in the spreadsheet
</commit_message>
<xml_diff>
--- a/segmentConstraints.xlsx
+++ b/segmentConstraints.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
   <si>
     <t>Parameter</t>
   </si>
@@ -101,12 +101,6 @@
   </si>
   <si>
     <t>N</t>
-  </si>
-  <si>
-    <t>True</t>
-  </si>
-  <si>
-    <t>False</t>
   </si>
 </sst>
 </file>
@@ -1780,7 +1774,7 @@
         <v>16</v>
       </c>
       <c r="B13" t="s" s="8">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="C13" t="s" s="10">
         <v>28</v>
@@ -1821,7 +1815,7 @@
         <v>16</v>
       </c>
       <c r="B14" t="s" s="8">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s" s="10">
         <v>28</v>
@@ -1862,7 +1856,7 @@
         <v>17</v>
       </c>
       <c r="B15" t="s" s="8">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s" s="10">
         <v>28</v>
@@ -1903,7 +1897,7 @@
         <v>17</v>
       </c>
       <c r="B16" t="s" s="8">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s" s="10">
         <v>28</v>

</xml_diff>

<commit_message>
Coding a Variation object to manage the variations from one set to the other.
</commit_message>
<xml_diff>
--- a/segmentConstraints.xlsx
+++ b/segmentConstraints.xlsx
@@ -188,7 +188,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -208,9 +208,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1398,46 +1395,48 @@
       <c r="L3" t="s" s="6">
         <v>26</v>
       </c>
-      <c r="M3" s="7"/>
+      <c r="M3" t="s" s="6">
+        <v>26</v>
+      </c>
     </row>
     <row r="4" ht="20.05" customHeight="1">
       <c r="A4" t="s" s="2">
         <v>13</v>
       </c>
-      <c r="B4" t="s" s="8">
+      <c r="B4" t="s" s="7">
         <v>18</v>
       </c>
-      <c r="C4" t="s" s="9">
-        <v>27</v>
-      </c>
-      <c r="D4" t="s" s="9">
-        <v>27</v>
-      </c>
-      <c r="E4" t="s" s="9">
-        <v>27</v>
-      </c>
-      <c r="F4" t="s" s="9">
-        <v>27</v>
-      </c>
-      <c r="G4" t="s" s="9">
-        <v>27</v>
-      </c>
-      <c r="H4" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="I4" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="J4" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="K4" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="L4" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="M4" t="s" s="10">
+      <c r="C4" t="s" s="8">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s" s="8">
+        <v>27</v>
+      </c>
+      <c r="E4" t="s" s="8">
+        <v>27</v>
+      </c>
+      <c r="F4" t="s" s="8">
+        <v>27</v>
+      </c>
+      <c r="G4" t="s" s="8">
+        <v>27</v>
+      </c>
+      <c r="H4" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="I4" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="J4" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="K4" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="L4" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="M4" t="s" s="9">
         <v>29</v>
       </c>
     </row>
@@ -1445,40 +1444,40 @@
       <c r="A5" t="s" s="2">
         <v>13</v>
       </c>
-      <c r="B5" t="s" s="8">
+      <c r="B5" t="s" s="7">
         <v>20</v>
       </c>
-      <c r="C5" t="s" s="9">
-        <v>27</v>
-      </c>
-      <c r="D5" t="s" s="9">
-        <v>27</v>
-      </c>
-      <c r="E5" t="s" s="9">
-        <v>27</v>
-      </c>
-      <c r="F5" t="s" s="9">
-        <v>27</v>
-      </c>
-      <c r="G5" t="s" s="9">
-        <v>27</v>
-      </c>
-      <c r="H5" t="s" s="10">
-        <v>29</v>
-      </c>
-      <c r="I5" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="J5" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="K5" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="L5" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="M5" t="s" s="10">
+      <c r="C5" t="s" s="8">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s" s="8">
+        <v>27</v>
+      </c>
+      <c r="E5" t="s" s="8">
+        <v>27</v>
+      </c>
+      <c r="F5" t="s" s="8">
+        <v>27</v>
+      </c>
+      <c r="G5" t="s" s="8">
+        <v>27</v>
+      </c>
+      <c r="H5" t="s" s="9">
+        <v>29</v>
+      </c>
+      <c r="I5" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="J5" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="K5" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="L5" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="M5" t="s" s="9">
         <v>29</v>
       </c>
     </row>
@@ -1486,40 +1485,40 @@
       <c r="A6" t="s" s="2">
         <v>13</v>
       </c>
-      <c r="B6" t="s" s="8">
+      <c r="B6" t="s" s="7">
         <v>19</v>
       </c>
-      <c r="C6" t="s" s="9">
-        <v>27</v>
-      </c>
-      <c r="D6" t="s" s="9">
-        <v>27</v>
-      </c>
-      <c r="E6" t="s" s="9">
-        <v>27</v>
-      </c>
-      <c r="F6" t="s" s="9">
-        <v>27</v>
-      </c>
-      <c r="G6" t="s" s="9">
-        <v>27</v>
-      </c>
-      <c r="H6" t="s" s="10">
-        <v>29</v>
-      </c>
-      <c r="I6" t="s" s="10">
-        <v>29</v>
-      </c>
-      <c r="J6" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="K6" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="L6" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="M6" t="s" s="10">
+      <c r="C6" t="s" s="8">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s" s="8">
+        <v>27</v>
+      </c>
+      <c r="E6" t="s" s="8">
+        <v>27</v>
+      </c>
+      <c r="F6" t="s" s="8">
+        <v>27</v>
+      </c>
+      <c r="G6" t="s" s="8">
+        <v>27</v>
+      </c>
+      <c r="H6" t="s" s="9">
+        <v>29</v>
+      </c>
+      <c r="I6" t="s" s="9">
+        <v>29</v>
+      </c>
+      <c r="J6" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="K6" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="L6" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="M6" t="s" s="9">
         <v>29</v>
       </c>
     </row>
@@ -1527,40 +1526,40 @@
       <c r="A7" t="s" s="2">
         <v>13</v>
       </c>
-      <c r="B7" t="s" s="8">
+      <c r="B7" t="s" s="7">
         <v>21</v>
       </c>
-      <c r="C7" t="s" s="9">
-        <v>27</v>
-      </c>
-      <c r="D7" t="s" s="9">
-        <v>27</v>
-      </c>
-      <c r="E7" t="s" s="9">
-        <v>27</v>
-      </c>
-      <c r="F7" t="s" s="9">
-        <v>27</v>
-      </c>
-      <c r="G7" t="s" s="9">
-        <v>27</v>
-      </c>
-      <c r="H7" t="s" s="10">
-        <v>29</v>
-      </c>
-      <c r="I7" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="J7" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="K7" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="L7" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="M7" t="s" s="10">
+      <c r="C7" t="s" s="8">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s" s="8">
+        <v>27</v>
+      </c>
+      <c r="E7" t="s" s="8">
+        <v>27</v>
+      </c>
+      <c r="F7" t="s" s="8">
+        <v>27</v>
+      </c>
+      <c r="G7" t="s" s="8">
+        <v>27</v>
+      </c>
+      <c r="H7" t="s" s="9">
+        <v>29</v>
+      </c>
+      <c r="I7" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="J7" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="K7" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="L7" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="M7" t="s" s="9">
         <v>29</v>
       </c>
     </row>
@@ -1568,40 +1567,40 @@
       <c r="A8" t="s" s="2">
         <v>13</v>
       </c>
-      <c r="B8" t="s" s="8">
+      <c r="B8" t="s" s="7">
         <v>22</v>
       </c>
-      <c r="C8" t="s" s="9">
-        <v>27</v>
-      </c>
-      <c r="D8" t="s" s="9">
-        <v>27</v>
-      </c>
-      <c r="E8" t="s" s="9">
-        <v>27</v>
-      </c>
-      <c r="F8" t="s" s="9">
-        <v>27</v>
-      </c>
-      <c r="G8" t="s" s="9">
-        <v>27</v>
-      </c>
-      <c r="H8" t="s" s="10">
-        <v>29</v>
-      </c>
-      <c r="I8" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="J8" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="K8" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="L8" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="M8" t="s" s="10">
+      <c r="C8" t="s" s="8">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s" s="8">
+        <v>27</v>
+      </c>
+      <c r="E8" t="s" s="8">
+        <v>27</v>
+      </c>
+      <c r="F8" t="s" s="8">
+        <v>27</v>
+      </c>
+      <c r="G8" t="s" s="8">
+        <v>27</v>
+      </c>
+      <c r="H8" t="s" s="9">
+        <v>29</v>
+      </c>
+      <c r="I8" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="J8" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="K8" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="L8" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="M8" t="s" s="9">
         <v>29</v>
       </c>
     </row>
@@ -1609,40 +1608,40 @@
       <c r="A9" t="s" s="2">
         <v>14</v>
       </c>
-      <c r="B9" t="s" s="8">
+      <c r="B9" t="s" s="7">
         <v>23</v>
       </c>
-      <c r="C9" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="D9" t="s" s="10">
-        <v>29</v>
-      </c>
-      <c r="E9" t="s" s="10">
-        <v>29</v>
-      </c>
-      <c r="F9" t="s" s="10">
-        <v>29</v>
-      </c>
-      <c r="G9" t="s" s="10">
-        <v>29</v>
-      </c>
-      <c r="H9" t="s" s="9">
-        <v>27</v>
-      </c>
-      <c r="I9" t="s" s="9">
-        <v>27</v>
-      </c>
-      <c r="J9" t="s" s="9">
-        <v>27</v>
-      </c>
-      <c r="K9" t="s" s="10">
-        <v>29</v>
-      </c>
-      <c r="L9" t="s" s="10">
-        <v>29</v>
-      </c>
-      <c r="M9" t="s" s="10">
+      <c r="C9" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="D9" t="s" s="9">
+        <v>29</v>
+      </c>
+      <c r="E9" t="s" s="9">
+        <v>29</v>
+      </c>
+      <c r="F9" t="s" s="9">
+        <v>29</v>
+      </c>
+      <c r="G9" t="s" s="9">
+        <v>29</v>
+      </c>
+      <c r="H9" t="s" s="8">
+        <v>27</v>
+      </c>
+      <c r="I9" t="s" s="8">
+        <v>27</v>
+      </c>
+      <c r="J9" t="s" s="8">
+        <v>27</v>
+      </c>
+      <c r="K9" t="s" s="9">
+        <v>29</v>
+      </c>
+      <c r="L9" t="s" s="9">
+        <v>29</v>
+      </c>
+      <c r="M9" t="s" s="9">
         <v>29</v>
       </c>
     </row>
@@ -1650,40 +1649,40 @@
       <c r="A10" t="s" s="2">
         <v>14</v>
       </c>
-      <c r="B10" t="s" s="8">
+      <c r="B10" t="s" s="7">
         <v>24</v>
       </c>
-      <c r="C10" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="D10" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="E10" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="F10" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="G10" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="H10" t="s" s="9">
-        <v>27</v>
-      </c>
-      <c r="I10" t="s" s="9">
-        <v>27</v>
-      </c>
-      <c r="J10" t="s" s="9">
-        <v>27</v>
-      </c>
-      <c r="K10" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="L10" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="M10" t="s" s="10">
+      <c r="C10" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="D10" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="E10" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="F10" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="G10" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="H10" t="s" s="8">
+        <v>27</v>
+      </c>
+      <c r="I10" t="s" s="8">
+        <v>27</v>
+      </c>
+      <c r="J10" t="s" s="8">
+        <v>27</v>
+      </c>
+      <c r="K10" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="L10" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="M10" t="s" s="9">
         <v>29</v>
       </c>
     </row>
@@ -1691,40 +1690,40 @@
       <c r="A11" t="s" s="2">
         <v>14</v>
       </c>
-      <c r="B11" t="s" s="8">
+      <c r="B11" t="s" s="7">
         <v>25</v>
       </c>
-      <c r="C11" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="D11" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="E11" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="F11" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="G11" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="H11" t="s" s="9">
-        <v>27</v>
-      </c>
-      <c r="I11" t="s" s="9">
-        <v>27</v>
-      </c>
-      <c r="J11" t="s" s="9">
-        <v>27</v>
-      </c>
-      <c r="K11" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="L11" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="M11" t="s" s="10">
+      <c r="C11" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="D11" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="E11" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="F11" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="G11" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="H11" t="s" s="8">
+        <v>27</v>
+      </c>
+      <c r="I11" t="s" s="8">
+        <v>27</v>
+      </c>
+      <c r="J11" t="s" s="8">
+        <v>27</v>
+      </c>
+      <c r="K11" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="L11" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="M11" t="s" s="9">
         <v>29</v>
       </c>
     </row>
@@ -1732,40 +1731,40 @@
       <c r="A12" t="s" s="2">
         <v>15</v>
       </c>
-      <c r="B12" t="s" s="8">
+      <c r="B12" t="s" s="7">
         <v>26</v>
       </c>
-      <c r="C12" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="D12" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="E12" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="F12" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="G12" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="H12" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="I12" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="J12" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="K12" t="s" s="9">
-        <v>27</v>
-      </c>
-      <c r="L12" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="M12" t="s" s="10">
+      <c r="C12" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="D12" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="E12" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="F12" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="G12" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="H12" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="I12" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="J12" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="K12" t="s" s="8">
+        <v>27</v>
+      </c>
+      <c r="L12" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="M12" t="s" s="9">
         <v>29</v>
       </c>
     </row>
@@ -1773,40 +1772,40 @@
       <c r="A13" t="s" s="2">
         <v>16</v>
       </c>
-      <c r="B13" t="s" s="8">
+      <c r="B13" t="s" s="7">
         <v>16</v>
       </c>
-      <c r="C13" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="D13" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="E13" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="F13" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="G13" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="H13" t="s" s="10">
-        <v>29</v>
-      </c>
-      <c r="I13" t="s" s="10">
-        <v>29</v>
-      </c>
-      <c r="J13" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="K13" t="s" s="10">
-        <v>29</v>
-      </c>
-      <c r="L13" t="s" s="9">
-        <v>27</v>
-      </c>
-      <c r="M13" t="s" s="10">
+      <c r="C13" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="D13" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="E13" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="F13" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="G13" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="H13" t="s" s="9">
+        <v>29</v>
+      </c>
+      <c r="I13" t="s" s="9">
+        <v>29</v>
+      </c>
+      <c r="J13" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="K13" t="s" s="9">
+        <v>29</v>
+      </c>
+      <c r="L13" t="s" s="8">
+        <v>27</v>
+      </c>
+      <c r="M13" t="s" s="9">
         <v>29</v>
       </c>
     </row>
@@ -1814,40 +1813,40 @@
       <c r="A14" t="s" s="2">
         <v>16</v>
       </c>
-      <c r="B14" t="s" s="8">
+      <c r="B14" t="s" s="7">
         <v>25</v>
       </c>
-      <c r="C14" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="D14" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="E14" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="F14" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="G14" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="H14" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="I14" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="J14" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="K14" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="L14" t="s" s="9">
-        <v>27</v>
-      </c>
-      <c r="M14" t="s" s="10">
+      <c r="C14" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="D14" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="E14" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="F14" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="G14" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="H14" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="I14" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="J14" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="K14" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="L14" t="s" s="8">
+        <v>27</v>
+      </c>
+      <c r="M14" t="s" s="9">
         <v>29</v>
       </c>
     </row>
@@ -1855,40 +1854,40 @@
       <c r="A15" t="s" s="2">
         <v>17</v>
       </c>
-      <c r="B15" t="s" s="8">
+      <c r="B15" t="s" s="7">
         <v>17</v>
       </c>
-      <c r="C15" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="D15" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="E15" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="F15" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="G15" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="H15" t="s" s="10">
-        <v>29</v>
-      </c>
-      <c r="I15" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="J15" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="K15" t="s" s="10">
-        <v>29</v>
-      </c>
-      <c r="L15" t="s" s="10">
-        <v>29</v>
-      </c>
-      <c r="M15" t="s" s="9">
+      <c r="C15" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="D15" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="E15" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="F15" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="G15" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="H15" t="s" s="9">
+        <v>29</v>
+      </c>
+      <c r="I15" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="J15" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="K15" t="s" s="9">
+        <v>29</v>
+      </c>
+      <c r="L15" t="s" s="9">
+        <v>29</v>
+      </c>
+      <c r="M15" t="s" s="8">
         <v>27</v>
       </c>
     </row>
@@ -1896,40 +1895,40 @@
       <c r="A16" t="s" s="2">
         <v>17</v>
       </c>
-      <c r="B16" t="s" s="8">
+      <c r="B16" t="s" s="7">
         <v>25</v>
       </c>
-      <c r="C16" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="D16" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="E16" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="F16" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="G16" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="H16" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="I16" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="J16" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="K16" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="L16" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="M16" t="s" s="9">
+      <c r="C16" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="D16" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="E16" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="F16" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="G16" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="H16" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="I16" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="J16" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="K16" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="L16" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="M16" t="s" s="8">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Chagne in the wording in the excel
</commit_message>
<xml_diff>
--- a/segmentConstraints.xlsx
+++ b/segmentConstraints.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="32">
   <si>
     <t>Parameter</t>
   </si>
@@ -88,7 +88,7 @@
     <t>fins</t>
   </si>
   <si>
-    <t>None</t>
+    <t>No equipment</t>
   </si>
   <si>
     <t>Any</t>
@@ -101,6 +101,12 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>No drill</t>
+  </si>
+  <si>
+    <t>No kick</t>
   </si>
 </sst>
 </file>
@@ -1814,7 +1820,7 @@
         <v>16</v>
       </c>
       <c r="B14" t="s" s="7">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s" s="9">
         <v>28</v>
@@ -1896,7 +1902,7 @@
         <v>17</v>
       </c>
       <c r="B16" t="s" s="7">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C16" t="s" s="9">
         <v>28</v>

</xml_diff>

<commit_message>
changing the constraints on the segments - variation. Being a bit more permissive with kick. We allowed kicks to vary from one segment to another.
</commit_message>
<xml_diff>
--- a/segmentConstraints.xlsx
+++ b/segmentConstraints.xlsx
@@ -1443,7 +1443,7 @@
         <v>28</v>
       </c>
       <c r="M4" t="s" s="9">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" ht="20.05" customHeight="1">
@@ -1484,7 +1484,7 @@
         <v>28</v>
       </c>
       <c r="M5" t="s" s="9">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" ht="20.05" customHeight="1">
@@ -1525,7 +1525,7 @@
         <v>28</v>
       </c>
       <c r="M6" t="s" s="9">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" ht="20.05" customHeight="1">
@@ -1566,7 +1566,7 @@
         <v>28</v>
       </c>
       <c r="M7" t="s" s="9">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" ht="20.05" customHeight="1">
@@ -1607,7 +1607,7 @@
         <v>28</v>
       </c>
       <c r="M8" t="s" s="9">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" ht="20.05" customHeight="1">
@@ -1642,10 +1642,10 @@
         <v>27</v>
       </c>
       <c r="K9" t="s" s="9">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L9" t="s" s="9">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M9" t="s" s="9">
         <v>29</v>
@@ -1689,7 +1689,7 @@
         <v>28</v>
       </c>
       <c r="M10" t="s" s="9">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" ht="20.05" customHeight="1">
@@ -1730,7 +1730,7 @@
         <v>28</v>
       </c>
       <c r="M11" t="s" s="9">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" ht="20.05" customHeight="1">
@@ -1771,7 +1771,7 @@
         <v>28</v>
       </c>
       <c r="M12" t="s" s="9">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" ht="20.05" customHeight="1">
@@ -1853,7 +1853,7 @@
         <v>27</v>
       </c>
       <c r="M14" t="s" s="9">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" ht="20.05" customHeight="1">
@@ -1888,7 +1888,7 @@
         <v>28</v>
       </c>
       <c r="K15" t="s" s="9">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L15" t="s" s="9">
         <v>29</v>

</xml_diff>